<commit_message>
Regression and Smoke Code changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestPack\WppRegPack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -300,13 +300,67 @@
   </si>
   <si>
     <t>TSTAUTO-1</t>
+  </si>
+  <si>
+    <t>CreateSubJob</t>
+  </si>
+  <si>
+    <t>PostVendorJournal</t>
+  </si>
+  <si>
+    <t>CreateExpenses</t>
+  </si>
+  <si>
+    <t>Approve_Expenses_Opco</t>
+  </si>
+  <si>
+    <t>Reject_Expenses</t>
+  </si>
+  <si>
+    <t>Post_a_Customer_Payment</t>
+  </si>
+  <si>
+    <t>Customer_Payment_for_Single_Invoice</t>
+  </si>
+  <si>
+    <t>Writing_Off_Bad_Debts</t>
+  </si>
+  <si>
+    <t>Create_Fixed_Asset</t>
+  </si>
+  <si>
+    <t>PostingAssetEntires</t>
+  </si>
+  <si>
+    <t>FixedAssetDisposal</t>
+  </si>
+  <si>
+    <t>FixedAssetReval</t>
+  </si>
+  <si>
+    <t>FixedAssetDepreciation</t>
+  </si>
+  <si>
+    <t>ChangeEmployee</t>
+  </si>
+  <si>
+    <t>CreateUser</t>
+  </si>
+  <si>
+    <t>ChangeUser</t>
+  </si>
+  <si>
+    <t>BlockUser</t>
+  </si>
+  <si>
+    <t>TSTAUTO7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +387,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -500,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -529,6 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1707</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,6 +1235,104 @@
       </c>
       <c r="C16" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1602,12 +1762,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1808,15 +1965,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1841,10 +2002,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added JIRA TestID in EnvParameters
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -354,6 +354,171 @@
   </si>
   <si>
     <t>TSTAUTO7</t>
+  </si>
+  <si>
+    <t>TSTAUTO44</t>
+  </si>
+  <si>
+    <t>TSTAUTO8</t>
+  </si>
+  <si>
+    <t>TSTAUTO46</t>
+  </si>
+  <si>
+    <t>TSTAUTO10</t>
+  </si>
+  <si>
+    <t>TSTAUTO50</t>
+  </si>
+  <si>
+    <t>TSTAUTO14</t>
+  </si>
+  <si>
+    <t>TSTAUTO47</t>
+  </si>
+  <si>
+    <t>TSTAUTO11</t>
+  </si>
+  <si>
+    <t>TSTAUTO49</t>
+  </si>
+  <si>
+    <t>TSTAUTO13</t>
+  </si>
+  <si>
+    <t>TSTAUTO48</t>
+  </si>
+  <si>
+    <t>TSTAUTO12</t>
+  </si>
+  <si>
+    <t>TSTAUTO62</t>
+  </si>
+  <si>
+    <t>TSTAUTO26</t>
+  </si>
+  <si>
+    <t>TSTAUTO63</t>
+  </si>
+  <si>
+    <t>TSTAUTO27</t>
+  </si>
+  <si>
+    <t>TSTAUTO64</t>
+  </si>
+  <si>
+    <t>TSTAUTO28</t>
+  </si>
+  <si>
+    <t>TSTAUTO39</t>
+  </si>
+  <si>
+    <t>TSTAUTO3</t>
+  </si>
+  <si>
+    <t>TSTAUTO56</t>
+  </si>
+  <si>
+    <t>TSTAUTO20</t>
+  </si>
+  <si>
+    <t>TSTAUTO55</t>
+  </si>
+  <si>
+    <t>TSTAUTO19</t>
+  </si>
+  <si>
+    <t>TSTAUTO40</t>
+  </si>
+  <si>
+    <t>TSTAUTO4</t>
+  </si>
+  <si>
+    <t>TSTAUTO42</t>
+  </si>
+  <si>
+    <t>TSTAUTO6</t>
+  </si>
+  <si>
+    <t>TSTAUTO43</t>
+  </si>
+  <si>
+    <t>TSTAUTO65</t>
+  </si>
+  <si>
+    <t>TSTAUTO29</t>
+  </si>
+  <si>
+    <t>TSTAUTO38</t>
+  </si>
+  <si>
+    <t>TSTAUTO2</t>
+  </si>
+  <si>
+    <t>TSTAUTO53</t>
+  </si>
+  <si>
+    <t>TSTAUTO17</t>
+  </si>
+  <si>
+    <t>TSTAUTO52</t>
+  </si>
+  <si>
+    <t>TSTAUTO16</t>
+  </si>
+  <si>
+    <t>TSTAUTO71</t>
+  </si>
+  <si>
+    <t>TSTAUTO35</t>
+  </si>
+  <si>
+    <t>TSTAUTO69</t>
+  </si>
+  <si>
+    <t>TSTAUTO33</t>
+  </si>
+  <si>
+    <t>TSTAUTO73</t>
+  </si>
+  <si>
+    <t>TSTAUTO37</t>
+  </si>
+  <si>
+    <t>TSTAUTO59</t>
+  </si>
+  <si>
+    <t>TSTAUTO23</t>
+  </si>
+  <si>
+    <t>TSTAUTO60</t>
+  </si>
+  <si>
+    <t>TSTAUTO24</t>
+  </si>
+  <si>
+    <t>TSTAUTO61</t>
+  </si>
+  <si>
+    <t>TSTAUTO25</t>
+  </si>
+  <si>
+    <t>TSTAUTO57</t>
+  </si>
+  <si>
+    <t>TSTAUTO21</t>
+  </si>
+  <si>
+    <t>TSTAUTO41</t>
+  </si>
+  <si>
+    <t>TSTAUTO5</t>
+  </si>
+  <si>
+    <t>TSTAUTO58</t>
+  </si>
+  <si>
+    <t>TSTAUTO22</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,160 +1252,163 @@
       <c r="A3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
+      <c r="B3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
+      <c r="B4" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
+      <c r="B5" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
+      <c r="B6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
+      <c r="B7" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
+      <c r="B8" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
+      <c r="B9" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
+      <c r="B10" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" t="s">
-        <v>89</v>
+      <c r="B11" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
+      <c r="B12" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>89</v>
+      <c r="B13" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
+      <c r="B14" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
+      <c r="B15" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>89</v>
+      <c r="B16" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>90</v>
       </c>
+      <c r="B17" s="18" t="s">
+        <v>136</v>
+      </c>
       <c r="C17" s="18" t="s">
         <v>107</v>
       </c>
@@ -1249,90 +1417,176 @@
       <c r="A18" s="17" t="s">
         <v>91</v>
       </c>
+      <c r="B18" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>92</v>
       </c>
+      <c r="B19" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>93</v>
       </c>
+      <c r="B20" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>94</v>
       </c>
+      <c r="B21" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>95</v>
       </c>
+      <c r="B22" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>96</v>
       </c>
+      <c r="B23" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>97</v>
       </c>
+      <c r="B24" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>98</v>
       </c>
+      <c r="B25" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>99</v>
       </c>
+      <c r="B26" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>100</v>
       </c>
+      <c r="B27" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>101</v>
       </c>
+      <c r="B28" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>102</v>
       </c>
+      <c r="B29" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>34</v>
+        <v>103</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>35</v>
+        <v>104</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
         <v>106</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1762,9 +2016,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1965,19 +2222,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2002,9 +2255,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding Block Global Client Script
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1307</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2016,9 +2016,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2219,19 +2222,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2256,9 +2255,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Jenkins Changes in scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="165">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -519,6 +519,12 @@
   </si>
   <si>
     <t>TSTAUTO-22</t>
+  </si>
+  <si>
+    <t>BlockGlobalClient</t>
+  </si>
+  <si>
+    <t>BlockGlobalBrand</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1100,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1707</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1179,9 +1185,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1206,6 +1212,11 @@
         <v>1307</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1214,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,6 +1597,28 @@
         <v>161</v>
       </c>
       <c r="C33" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Script Changes - Vendor Management , Client Management(Company related) . DataSheet Changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="182">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -1101,7 +1101,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,6 +1808,9 @@
       </c>
       <c r="B44" s="18" t="s">
         <v>176</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>159</v>
       </c>
       <c r="D44" t="s">
         <v>179</v>
@@ -2122,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,9 +2256,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2456,19 +2462,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2493,9 +2495,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Made changes To Run Manager and Environment Parameters/
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="217">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -560,9 +560,6 @@
     <t>CreateClient</t>
   </si>
   <si>
-    <t>TSTAUTO-77</t>
-  </si>
-  <si>
     <t>Singapore</t>
   </si>
   <si>
@@ -576,6 +573,114 @@
   </si>
   <si>
     <t>TSTAUTO-92</t>
+  </si>
+  <si>
+    <t>CreateGlobalBrand</t>
+  </si>
+  <si>
+    <t>CreateGlobalProduct</t>
+  </si>
+  <si>
+    <t>CreateCompanyClient</t>
+  </si>
+  <si>
+    <t>CreateCompanyBrand</t>
+  </si>
+  <si>
+    <t>CreateCompanyProduct</t>
+  </si>
+  <si>
+    <t>CreateGlobalVendor</t>
+  </si>
+  <si>
+    <t>CompanyVendor</t>
+  </si>
+  <si>
+    <t>AmendComapnyVendor</t>
+  </si>
+  <si>
+    <t>AmendGlobalVendor</t>
+  </si>
+  <si>
+    <t>AmendCompanyProduct</t>
+  </si>
+  <si>
+    <t>AmendCompanyBrand</t>
+  </si>
+  <si>
+    <t>AmendCompanyClient</t>
+  </si>
+  <si>
+    <t>AmendGlobalProduct</t>
+  </si>
+  <si>
+    <t>TSTAUTO-96</t>
+  </si>
+  <si>
+    <t>TSTAUTO-91</t>
+  </si>
+  <si>
+    <t>TSTAUTO-94</t>
+  </si>
+  <si>
+    <t>TSTAUTO-90</t>
+  </si>
+  <si>
+    <t>TSTAUTO-85</t>
+  </si>
+  <si>
+    <t>TSTAUTO-78</t>
+  </si>
+  <si>
+    <t>TSTAUTO-97</t>
+  </si>
+  <si>
+    <t>TSTAUTO-98</t>
+  </si>
+  <si>
+    <t>TSTAUTO-99</t>
+  </si>
+  <si>
+    <t>TSTAUTO-100</t>
+  </si>
+  <si>
+    <t>TSTAUTO-101</t>
+  </si>
+  <si>
+    <t>TSTAUTO-102</t>
+  </si>
+  <si>
+    <t>TSTAUTO-103</t>
+  </si>
+  <si>
+    <t>TSTAUTO-104</t>
+  </si>
+  <si>
+    <t>TSTAUTO-105</t>
+  </si>
+  <si>
+    <t>TSTAUTO-107</t>
+  </si>
+  <si>
+    <t>TSTAUTO-108</t>
+  </si>
+  <si>
+    <t>TSTAUTO-109</t>
+  </si>
+  <si>
+    <t>TSTAUTO-110</t>
+  </si>
+  <si>
+    <t>TSTAUTO-111</t>
+  </si>
+  <si>
+    <t>TSTAUTO-112</t>
+  </si>
+  <si>
+    <t>TSTAUTO-114</t>
+  </si>
+  <si>
+    <t>TSTAUTO-113</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1368,7 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,16 +1413,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1331,7 +1437,7 @@
         <v>39</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,55 +1793,55 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="17" t="s">
         <v>160</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="17" t="s">
         <v>161</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>162</v>
+      <c r="A36" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>164</v>
+      <c r="A37" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>165</v>
+      <c r="A38" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>159</v>
@@ -1743,10 +1849,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>159</v>
@@ -1754,66 +1860,209 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>159</v>
       </c>
+      <c r="D40" s="18" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>159</v>
       </c>
+      <c r="D41" s="18" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>169</v>
+      <c r="A42" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>170</v>
-      </c>
       <c r="B43" s="18" t="s">
-        <v>158</v>
+        <v>200</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>175</v>
+      <c r="A44" s="17" t="s">
+        <v>182</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D44" t="s">
-        <v>179</v>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Amended Code for Company Client, Brand and Vendor
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,6 +2505,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2513,7 +2519,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -2710,13 +2716,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2724,7 +2733,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E10866D-5BB4-44E5-B346-014C2F2BBDD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2741,13 +2750,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Company Vendor Changes + Datasheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -641,9 +641,6 @@
     <t>TSTAUTO-99</t>
   </si>
   <si>
-    <t>TSTAUTO-100</t>
-  </si>
-  <si>
     <t>TSTAUTO-101</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>TSTAUTO-113</t>
+  </si>
+  <si>
+    <t>TSTAUTO-115</t>
   </si>
 </sst>
 </file>
@@ -1415,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1830,7 @@
         <v>165</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>159</v>
@@ -1841,7 +1841,7 @@
         <v>166</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>159</v>
@@ -1927,7 +1927,7 @@
         <v>183</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>159</v>
@@ -1938,7 +1938,7 @@
         <v>184</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>159</v>
@@ -1949,7 +1949,7 @@
         <v>185</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>159</v>
@@ -1971,7 +1971,7 @@
         <v>187</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>159</v>
@@ -1982,7 +1982,7 @@
         <v>188</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>159</v>
@@ -1993,7 +1993,7 @@
         <v>189</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>159</v>
@@ -2004,7 +2004,7 @@
         <v>168</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>159</v>
@@ -2015,7 +2015,7 @@
         <v>162</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>159</v>
@@ -2026,7 +2026,7 @@
         <v>190</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>159</v>
@@ -2037,7 +2037,7 @@
         <v>191</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>159</v>
@@ -2048,7 +2048,7 @@
         <v>192</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>159</v>
@@ -2059,7 +2059,7 @@
         <v>193</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>159</v>
@@ -2505,6 +2505,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -2701,22 +2716,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E10866D-5BB4-44E5-B346-014C2F2BBDD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2733,21 +2758,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DataSheet and TestRunner,EnvParams,JIRA,EventHandler script updation for JIRA.
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="224">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -687,6 +687,21 @@
   </si>
   <si>
     <t>CreateAGeneralJournal</t>
+  </si>
+  <si>
+    <t>Current Release Name</t>
+  </si>
+  <si>
+    <t>Release 2</t>
+  </si>
+  <si>
+    <t>Current Cycle Name</t>
+  </si>
+  <si>
+    <t>ReverseAGeneralJournal</t>
+  </si>
+  <si>
+    <t>TSTAUTO-117</t>
   </si>
 </sst>
 </file>
@@ -752,7 +767,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -889,12 +904,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -928,6 +958,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1419,17 +1452,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,294 +1481,296 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
+      <c r="A2" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>107</v>
+      <c r="A3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>109</v>
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>150</v>
@@ -1745,65 +1781,65 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>159</v>
@@ -1811,10 +1847,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>159</v>
@@ -1822,10 +1858,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>159</v>
@@ -1833,10 +1869,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>159</v>
@@ -1844,10 +1880,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>159</v>
@@ -1855,10 +1891,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>159</v>
@@ -1866,74 +1902,74 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D42" t="s">
-        <v>178</v>
+      <c r="D42" s="18" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>159</v>
       </c>
+      <c r="D43" s="18" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>159</v>
       </c>
+      <c r="D44" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>159</v>
@@ -1941,10 +1977,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>159</v>
@@ -1952,10 +1988,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>159</v>
@@ -1963,123 +1999,156 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D60" s="23" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2522,6 +2591,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -2718,22 +2802,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E10866D-5BB4-44E5-B346-014C2F2BBDD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2750,29 +2844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EnvParamaters.xlsx - changes for JIRA
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\3D Objects\GIT project\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="234">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -113,15 +113,9 @@
     <t>CORE - Test Automation</t>
   </si>
   <si>
-    <t>VersionName</t>
-  </si>
-  <si>
     <t>Release 1</t>
   </si>
   <si>
-    <t>CycleName</t>
-  </si>
-  <si>
     <t>Test Summary</t>
   </si>
   <si>
@@ -714,6 +708,30 @@
   </si>
   <si>
     <t>InvoicePreparation</t>
+  </si>
+  <si>
+    <t>JIRA User Name</t>
+  </si>
+  <si>
+    <t>JIRA Access Key</t>
+  </si>
+  <si>
+    <t>JIRA Secret Key</t>
+  </si>
+  <si>
+    <t>Zephyr BaseUrl</t>
+  </si>
+  <si>
+    <t>muthukumar.m@cognizant.com</t>
+  </si>
+  <si>
+    <t>MDA1MDIyZWQtZmEyMC0zOTc4LWI2ZmEtZDM3MTcxMGU1YzRjIDVjYjc1OTJmOWE4NTc5MTA4OTZmZTc5OSBVU0VSX0RFRkFVTFRfTkFNRQ</t>
+  </si>
+  <si>
+    <t>jf9LV-GHNp6MKw35xCTPo43WC0V4bwYC4SdsZC5K-Ho</t>
+  </si>
+  <si>
+    <t>https://prod-api.zephyr4jiracloud.com/connect</t>
   </si>
 </sst>
 </file>
@@ -936,7 +954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -973,6 +991,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1254,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,20 +1348,44 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8"/>
+      <c r="A8" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>233</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B9:B11" r:id="rId2" display="muthukumar.m@cognizant.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1357,7 +1406,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>12</v>
@@ -1366,18 +1415,18 @@
         <v>16</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -1386,21 +1435,21 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1421,19 +1470,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,7 +1532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
@@ -1497,698 +1546,698 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2215,7 +2264,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2223,7 +2272,7 @@
         <v>1201</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2231,7 +2280,7 @@
         <v>1322</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2239,7 +2288,7 @@
         <v>1314</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,7 +2296,7 @@
         <v>1319</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2255,7 +2304,7 @@
         <v>1307</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,7 +2312,7 @@
         <v>1204</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2271,7 +2320,7 @@
         <v>1213</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2279,7 +2328,7 @@
         <v>1284</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2336,7 @@
         <v>1271</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2295,7 +2344,7 @@
         <v>1205</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2303,7 +2352,7 @@
         <v>1240</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2360,7 @@
         <v>1228</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2368,7 @@
         <v>1315</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,7 +2376,7 @@
         <v>1309</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2335,7 +2384,7 @@
         <v>1318</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2343,7 +2392,7 @@
         <v>1321</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2351,7 +2400,7 @@
         <v>1301</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2359,7 +2408,7 @@
         <v>1295</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,7 +2416,7 @@
         <v>1289</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2375,7 +2424,7 @@
         <v>1216</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2383,7 +2432,7 @@
         <v>1285</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2391,7 +2440,7 @@
         <v>1273</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,7 +2448,7 @@
         <v>1269</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,7 +2456,7 @@
         <v>1263</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2464,7 @@
         <v>1221</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,7 +2472,7 @@
         <v>1253</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2480,7 @@
         <v>1203</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2439,7 +2488,7 @@
         <v>1246</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2447,7 +2496,7 @@
         <v>1229</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2504,7 @@
         <v>1239</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2512,7 @@
         <v>1296</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2520,7 @@
         <v>1304</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2528,7 @@
         <v>1214</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2536,7 @@
         <v>1330</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2574,7 +2623,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2588,7 +2637,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2616,7 +2665,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2640,12 +2689,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -2842,6 +2885,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
@@ -2851,23 +2900,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E10866D-5BB4-44E5-B346-014C2F2BBDD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2884,4 +2916,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EnvParamaters.xlsx, IND_Regression sheet changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Demo\Demo1\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Music\GIT_ProjectLatest\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -592,9 +592,6 @@
     <t>SPAIN</t>
   </si>
   <si>
-    <t>InvoicePreparation</t>
-  </si>
-  <si>
     <t>JIRA User Name</t>
   </si>
   <si>
@@ -628,9 +625,6 @@
     <t>InvoiceOnAccount</t>
   </si>
   <si>
-    <t>InvoicingFromBudget</t>
-  </si>
-  <si>
     <t>Partial_invoicing_WriteOff</t>
   </si>
   <si>
@@ -647,6 +641,12 @@
   </si>
   <si>
     <t>TSTAUTO-118</t>
+  </si>
+  <si>
+    <t>Invoicing from Budget</t>
+  </si>
+  <si>
+    <t>Invoice Preparation - Transfer Budget to Invoice On Account</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,34 +1264,34 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1337,7 @@
         <v>185</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1376,10 +1376,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1465,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2317,10 +2317,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>122</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>175</v>
@@ -2345,44 +2345,44 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Absence and Fixed Asset
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Script Fixing\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -8087,7 +8087,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8109,7 +8109,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -10213,2394 +10213,2394 @@
   </sheetData>
   <autoFilter ref="A1:E100"/>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="735" priority="729">
+    <cfRule type="expression" dxfId="767" priority="729">
       <formula>$L3="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="734" priority="730">
+    <cfRule type="expression" dxfId="766" priority="730">
       <formula>$L3="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="733" priority="731">
+    <cfRule type="expression" dxfId="765" priority="731">
       <formula>$L3="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="732" priority="732">
+    <cfRule type="expression" dxfId="764" priority="732">
       <formula>$L3="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="731" priority="733">
+    <cfRule type="expression" dxfId="763" priority="733">
       <formula>$L3="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="730" priority="734">
+    <cfRule type="expression" dxfId="762" priority="734">
       <formula>$L3="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="729" priority="735">
+    <cfRule type="expression" dxfId="761" priority="735">
       <formula>$L3="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="728" priority="736">
+    <cfRule type="expression" dxfId="760" priority="736">
       <formula>$L3="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="727" priority="721">
+    <cfRule type="expression" dxfId="759" priority="721">
       <formula>$L4="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="726" priority="722">
+    <cfRule type="expression" dxfId="758" priority="722">
       <formula>$L4="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="725" priority="723">
+    <cfRule type="expression" dxfId="757" priority="723">
       <formula>$L4="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="724" priority="724">
+    <cfRule type="expression" dxfId="756" priority="724">
       <formula>$L4="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="723" priority="725">
+    <cfRule type="expression" dxfId="755" priority="725">
       <formula>$L4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="722" priority="726">
+    <cfRule type="expression" dxfId="754" priority="726">
       <formula>$L4="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="721" priority="727">
+    <cfRule type="expression" dxfId="753" priority="727">
       <formula>$L4="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="720" priority="728">
+    <cfRule type="expression" dxfId="752" priority="728">
       <formula>$L4="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:B44">
-    <cfRule type="expression" dxfId="719" priority="713">
+    <cfRule type="expression" dxfId="751" priority="713">
       <formula>$L43="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="718" priority="714">
+    <cfRule type="expression" dxfId="750" priority="714">
       <formula>$L43="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="717" priority="715">
+    <cfRule type="expression" dxfId="749" priority="715">
       <formula>$L43="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="716" priority="716">
+    <cfRule type="expression" dxfId="748" priority="716">
       <formula>$L43="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="715" priority="717">
+    <cfRule type="expression" dxfId="747" priority="717">
       <formula>$L43="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="714" priority="718">
+    <cfRule type="expression" dxfId="746" priority="718">
       <formula>$L43="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="713" priority="719">
+    <cfRule type="expression" dxfId="745" priority="719">
       <formula>$L43="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="712" priority="720">
+    <cfRule type="expression" dxfId="744" priority="720">
       <formula>$L43="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" dxfId="711" priority="609">
+    <cfRule type="expression" dxfId="743" priority="609">
       <formula>$L98="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="710" priority="610">
+    <cfRule type="expression" dxfId="742" priority="610">
       <formula>$L98="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="709" priority="611">
+    <cfRule type="expression" dxfId="741" priority="611">
       <formula>$L98="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="708" priority="612">
+    <cfRule type="expression" dxfId="740" priority="612">
       <formula>$L98="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="707" priority="613">
+    <cfRule type="expression" dxfId="739" priority="613">
       <formula>$L98="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="706" priority="614">
+    <cfRule type="expression" dxfId="738" priority="614">
       <formula>$L98="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="705" priority="615">
+    <cfRule type="expression" dxfId="737" priority="615">
       <formula>$L98="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="704" priority="616">
+    <cfRule type="expression" dxfId="736" priority="616">
       <formula>$L98="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="expression" dxfId="703" priority="705">
+    <cfRule type="expression" dxfId="735" priority="705">
       <formula>$L70="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="702" priority="706">
+    <cfRule type="expression" dxfId="734" priority="706">
       <formula>$L70="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="701" priority="707">
+    <cfRule type="expression" dxfId="733" priority="707">
       <formula>$L70="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="700" priority="708">
+    <cfRule type="expression" dxfId="732" priority="708">
       <formula>$L70="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="699" priority="709">
+    <cfRule type="expression" dxfId="731" priority="709">
       <formula>$L70="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="698" priority="710">
+    <cfRule type="expression" dxfId="730" priority="710">
       <formula>$L70="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="697" priority="711">
+    <cfRule type="expression" dxfId="729" priority="711">
       <formula>$L70="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="696" priority="712">
+    <cfRule type="expression" dxfId="728" priority="712">
       <formula>$L70="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="expression" dxfId="695" priority="697">
+    <cfRule type="expression" dxfId="727" priority="697">
       <formula>$L76="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="694" priority="698">
+    <cfRule type="expression" dxfId="726" priority="698">
       <formula>$L76="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="693" priority="699">
+    <cfRule type="expression" dxfId="725" priority="699">
       <formula>$L76="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="692" priority="700">
+    <cfRule type="expression" dxfId="724" priority="700">
       <formula>$L76="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="691" priority="701">
+    <cfRule type="expression" dxfId="723" priority="701">
       <formula>$L76="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="690" priority="702">
+    <cfRule type="expression" dxfId="722" priority="702">
       <formula>$L76="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="689" priority="703">
+    <cfRule type="expression" dxfId="721" priority="703">
       <formula>$L76="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="688" priority="704">
+    <cfRule type="expression" dxfId="720" priority="704">
       <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B81">
-    <cfRule type="expression" dxfId="687" priority="689">
+    <cfRule type="expression" dxfId="719" priority="689">
       <formula>$L77="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="686" priority="690">
+    <cfRule type="expression" dxfId="718" priority="690">
       <formula>$L77="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="685" priority="691">
+    <cfRule type="expression" dxfId="717" priority="691">
       <formula>$L77="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="684" priority="692">
+    <cfRule type="expression" dxfId="716" priority="692">
       <formula>$L77="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="683" priority="693">
+    <cfRule type="expression" dxfId="715" priority="693">
       <formula>$L77="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="682" priority="694">
+    <cfRule type="expression" dxfId="714" priority="694">
       <formula>$L77="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="681" priority="695">
+    <cfRule type="expression" dxfId="713" priority="695">
       <formula>$L77="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="680" priority="696">
+    <cfRule type="expression" dxfId="712" priority="696">
       <formula>$L77="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B87">
-    <cfRule type="expression" dxfId="679" priority="681">
+    <cfRule type="expression" dxfId="711" priority="681">
       <formula>$L82="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="678" priority="682">
+    <cfRule type="expression" dxfId="710" priority="682">
       <formula>$L82="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="677" priority="683">
+    <cfRule type="expression" dxfId="709" priority="683">
       <formula>$L82="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="676" priority="684">
+    <cfRule type="expression" dxfId="708" priority="684">
       <formula>$L82="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="675" priority="685">
+    <cfRule type="expression" dxfId="707" priority="685">
       <formula>$L82="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="674" priority="686">
+    <cfRule type="expression" dxfId="706" priority="686">
       <formula>$L82="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="673" priority="687">
+    <cfRule type="expression" dxfId="705" priority="687">
       <formula>$L82="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="672" priority="688">
+    <cfRule type="expression" dxfId="704" priority="688">
       <formula>$L82="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="671" priority="673">
+    <cfRule type="expression" dxfId="703" priority="673">
       <formula>$L88="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="670" priority="674">
+    <cfRule type="expression" dxfId="702" priority="674">
       <formula>$L88="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="669" priority="675">
+    <cfRule type="expression" dxfId="701" priority="675">
       <formula>$L88="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="668" priority="676">
+    <cfRule type="expression" dxfId="700" priority="676">
       <formula>$L88="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="667" priority="677">
+    <cfRule type="expression" dxfId="699" priority="677">
       <formula>$L88="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="666" priority="678">
+    <cfRule type="expression" dxfId="698" priority="678">
       <formula>$L88="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="665" priority="679">
+    <cfRule type="expression" dxfId="697" priority="679">
       <formula>$L88="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="664" priority="680">
+    <cfRule type="expression" dxfId="696" priority="680">
       <formula>$L88="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" dxfId="663" priority="665">
+    <cfRule type="expression" dxfId="695" priority="665">
       <formula>$L89="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="662" priority="666">
+    <cfRule type="expression" dxfId="694" priority="666">
       <formula>$L89="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="661" priority="667">
+    <cfRule type="expression" dxfId="693" priority="667">
       <formula>$L89="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="660" priority="668">
+    <cfRule type="expression" dxfId="692" priority="668">
       <formula>$L89="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="659" priority="669">
+    <cfRule type="expression" dxfId="691" priority="669">
       <formula>$L89="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="658" priority="670">
+    <cfRule type="expression" dxfId="690" priority="670">
       <formula>$L89="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="657" priority="671">
+    <cfRule type="expression" dxfId="689" priority="671">
       <formula>$L89="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="656" priority="672">
+    <cfRule type="expression" dxfId="688" priority="672">
       <formula>$L89="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="655" priority="657">
+    <cfRule type="expression" dxfId="687" priority="657">
       <formula>$L90="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="654" priority="658">
+    <cfRule type="expression" dxfId="686" priority="658">
       <formula>$L90="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="653" priority="659">
+    <cfRule type="expression" dxfId="685" priority="659">
       <formula>$L90="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="652" priority="660">
+    <cfRule type="expression" dxfId="684" priority="660">
       <formula>$L90="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="651" priority="661">
+    <cfRule type="expression" dxfId="683" priority="661">
       <formula>$L90="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="650" priority="662">
+    <cfRule type="expression" dxfId="682" priority="662">
       <formula>$L90="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="649" priority="663">
+    <cfRule type="expression" dxfId="681" priority="663">
       <formula>$L90="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="648" priority="664">
+    <cfRule type="expression" dxfId="680" priority="664">
       <formula>$L90="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="647" priority="649">
+    <cfRule type="expression" dxfId="679" priority="649">
       <formula>$L91="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="646" priority="650">
+    <cfRule type="expression" dxfId="678" priority="650">
       <formula>$L91="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="645" priority="651">
+    <cfRule type="expression" dxfId="677" priority="651">
       <formula>$L91="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="644" priority="652">
+    <cfRule type="expression" dxfId="676" priority="652">
       <formula>$L91="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="643" priority="653">
+    <cfRule type="expression" dxfId="675" priority="653">
       <formula>$L91="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="642" priority="654">
+    <cfRule type="expression" dxfId="674" priority="654">
       <formula>$L91="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="641" priority="655">
+    <cfRule type="expression" dxfId="673" priority="655">
       <formula>$L91="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="640" priority="656">
+    <cfRule type="expression" dxfId="672" priority="656">
       <formula>$L91="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="639" priority="641">
+    <cfRule type="expression" dxfId="671" priority="641">
       <formula>$L92="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="638" priority="642">
+    <cfRule type="expression" dxfId="670" priority="642">
       <formula>$L92="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="637" priority="643">
+    <cfRule type="expression" dxfId="669" priority="643">
       <formula>$L92="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="636" priority="644">
+    <cfRule type="expression" dxfId="668" priority="644">
       <formula>$L92="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="635" priority="645">
+    <cfRule type="expression" dxfId="667" priority="645">
       <formula>$L92="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="634" priority="646">
+    <cfRule type="expression" dxfId="666" priority="646">
       <formula>$L92="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="633" priority="647">
+    <cfRule type="expression" dxfId="665" priority="647">
       <formula>$L92="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="632" priority="648">
+    <cfRule type="expression" dxfId="664" priority="648">
       <formula>$L92="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="631" priority="633">
+    <cfRule type="expression" dxfId="663" priority="633">
       <formula>$L93="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="630" priority="634">
+    <cfRule type="expression" dxfId="662" priority="634">
       <formula>$L93="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="629" priority="635">
+    <cfRule type="expression" dxfId="661" priority="635">
       <formula>$L93="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="628" priority="636">
+    <cfRule type="expression" dxfId="660" priority="636">
       <formula>$L93="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="627" priority="637">
+    <cfRule type="expression" dxfId="659" priority="637">
       <formula>$L93="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="626" priority="638">
+    <cfRule type="expression" dxfId="658" priority="638">
       <formula>$L93="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="625" priority="639">
+    <cfRule type="expression" dxfId="657" priority="639">
       <formula>$L93="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="624" priority="640">
+    <cfRule type="expression" dxfId="656" priority="640">
       <formula>$L93="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94:B96">
-    <cfRule type="expression" dxfId="623" priority="625">
+    <cfRule type="expression" dxfId="655" priority="625">
       <formula>$L94="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="622" priority="626">
+    <cfRule type="expression" dxfId="654" priority="626">
       <formula>$L94="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="621" priority="627">
+    <cfRule type="expression" dxfId="653" priority="627">
       <formula>$L94="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="620" priority="628">
+    <cfRule type="expression" dxfId="652" priority="628">
       <formula>$L94="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="619" priority="629">
+    <cfRule type="expression" dxfId="651" priority="629">
       <formula>$L94="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="618" priority="630">
+    <cfRule type="expression" dxfId="650" priority="630">
       <formula>$L94="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="617" priority="631">
+    <cfRule type="expression" dxfId="649" priority="631">
       <formula>$L94="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="616" priority="632">
+    <cfRule type="expression" dxfId="648" priority="632">
       <formula>$L94="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" dxfId="615" priority="617">
+    <cfRule type="expression" dxfId="647" priority="617">
       <formula>$L97="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="614" priority="618">
+    <cfRule type="expression" dxfId="646" priority="618">
       <formula>$L97="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="613" priority="619">
+    <cfRule type="expression" dxfId="645" priority="619">
       <formula>$L97="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="612" priority="620">
+    <cfRule type="expression" dxfId="644" priority="620">
       <formula>$L97="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="611" priority="621">
+    <cfRule type="expression" dxfId="643" priority="621">
       <formula>$L97="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="610" priority="622">
+    <cfRule type="expression" dxfId="642" priority="622">
       <formula>$L97="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="609" priority="623">
+    <cfRule type="expression" dxfId="641" priority="623">
       <formula>$L97="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="608" priority="624">
+    <cfRule type="expression" dxfId="640" priority="624">
       <formula>$L97="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:B11">
-    <cfRule type="expression" dxfId="607" priority="601">
+    <cfRule type="expression" dxfId="639" priority="601">
       <formula>$L9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="606" priority="602">
+    <cfRule type="expression" dxfId="638" priority="602">
       <formula>$L9="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="605" priority="603">
+    <cfRule type="expression" dxfId="637" priority="603">
       <formula>$L9="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="604" priority="604">
+    <cfRule type="expression" dxfId="636" priority="604">
       <formula>$L9="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="603" priority="605">
+    <cfRule type="expression" dxfId="635" priority="605">
       <formula>$L9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="602" priority="606">
+    <cfRule type="expression" dxfId="634" priority="606">
       <formula>$L9="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="601" priority="607">
+    <cfRule type="expression" dxfId="633" priority="607">
       <formula>$L9="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="600" priority="608">
+    <cfRule type="expression" dxfId="632" priority="608">
       <formula>$L9="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:B17">
-    <cfRule type="expression" dxfId="599" priority="593">
+    <cfRule type="expression" dxfId="631" priority="593">
       <formula>$L17="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="598" priority="594">
+    <cfRule type="expression" dxfId="630" priority="594">
       <formula>$L17="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="597" priority="595">
+    <cfRule type="expression" dxfId="629" priority="595">
       <formula>$L17="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="596" priority="596">
+    <cfRule type="expression" dxfId="628" priority="596">
       <formula>$L17="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="595" priority="597">
+    <cfRule type="expression" dxfId="627" priority="597">
       <formula>$L17="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="594" priority="598">
+    <cfRule type="expression" dxfId="626" priority="598">
       <formula>$L17="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="593" priority="599">
+    <cfRule type="expression" dxfId="625" priority="599">
       <formula>$L17="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="592" priority="600">
+    <cfRule type="expression" dxfId="624" priority="600">
       <formula>$L17="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29">
-    <cfRule type="expression" dxfId="591" priority="585">
+    <cfRule type="expression" dxfId="623" priority="585">
       <formula>$L29="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="590" priority="586">
+    <cfRule type="expression" dxfId="622" priority="586">
       <formula>$L29="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="589" priority="587">
+    <cfRule type="expression" dxfId="621" priority="587">
       <formula>$L29="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="588" priority="588">
+    <cfRule type="expression" dxfId="620" priority="588">
       <formula>$L29="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="587" priority="589">
+    <cfRule type="expression" dxfId="619" priority="589">
       <formula>$L29="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="586" priority="590">
+    <cfRule type="expression" dxfId="618" priority="590">
       <formula>$L29="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="585" priority="591">
+    <cfRule type="expression" dxfId="617" priority="591">
       <formula>$L29="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="584" priority="592">
+    <cfRule type="expression" dxfId="616" priority="592">
       <formula>$L29="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33">
-    <cfRule type="expression" dxfId="583" priority="577">
+    <cfRule type="expression" dxfId="615" priority="577">
       <formula>$L33="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="582" priority="578">
+    <cfRule type="expression" dxfId="614" priority="578">
       <formula>$L33="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="581" priority="579">
+    <cfRule type="expression" dxfId="613" priority="579">
       <formula>$L33="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="580" priority="580">
+    <cfRule type="expression" dxfId="612" priority="580">
       <formula>$L33="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="579" priority="581">
+    <cfRule type="expression" dxfId="611" priority="581">
       <formula>$L33="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="578" priority="582">
+    <cfRule type="expression" dxfId="610" priority="582">
       <formula>$L33="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="577" priority="583">
+    <cfRule type="expression" dxfId="609" priority="583">
       <formula>$L33="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="576" priority="584">
+    <cfRule type="expression" dxfId="608" priority="584">
       <formula>$L33="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B36">
-    <cfRule type="expression" dxfId="575" priority="561">
+    <cfRule type="expression" dxfId="607" priority="561">
       <formula>$L36="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="574" priority="562">
+    <cfRule type="expression" dxfId="606" priority="562">
       <formula>$L36="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="573" priority="563">
+    <cfRule type="expression" dxfId="605" priority="563">
       <formula>$L36="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="572" priority="564">
+    <cfRule type="expression" dxfId="604" priority="564">
       <formula>$L36="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="571" priority="565">
+    <cfRule type="expression" dxfId="603" priority="565">
       <formula>$L36="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="570" priority="566">
+    <cfRule type="expression" dxfId="602" priority="566">
       <formula>$L36="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="569" priority="567">
+    <cfRule type="expression" dxfId="601" priority="567">
       <formula>$L36="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="568" priority="568">
+    <cfRule type="expression" dxfId="600" priority="568">
       <formula>$L36="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B35">
-    <cfRule type="expression" dxfId="567" priority="569">
+    <cfRule type="expression" dxfId="599" priority="569">
       <formula>$L35="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="566" priority="570">
+    <cfRule type="expression" dxfId="598" priority="570">
       <formula>$L35="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="565" priority="571">
+    <cfRule type="expression" dxfId="597" priority="571">
       <formula>$L35="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="564" priority="572">
+    <cfRule type="expression" dxfId="596" priority="572">
       <formula>$L35="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="563" priority="573">
+    <cfRule type="expression" dxfId="595" priority="573">
       <formula>$L35="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="562" priority="574">
+    <cfRule type="expression" dxfId="594" priority="574">
       <formula>$L35="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="561" priority="575">
+    <cfRule type="expression" dxfId="593" priority="575">
       <formula>$L35="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="560" priority="576">
+    <cfRule type="expression" dxfId="592" priority="576">
       <formula>$L35="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B56">
-    <cfRule type="expression" dxfId="559" priority="553">
+    <cfRule type="expression" dxfId="591" priority="553">
       <formula>$L56="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="558" priority="554">
+    <cfRule type="expression" dxfId="590" priority="554">
       <formula>$L56="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="557" priority="555">
+    <cfRule type="expression" dxfId="589" priority="555">
       <formula>$L56="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="556" priority="556">
+    <cfRule type="expression" dxfId="588" priority="556">
       <formula>$L56="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="555" priority="557">
+    <cfRule type="expression" dxfId="587" priority="557">
       <formula>$L56="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="554" priority="558">
+    <cfRule type="expression" dxfId="586" priority="558">
       <formula>$L56="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="553" priority="559">
+    <cfRule type="expression" dxfId="585" priority="559">
       <formula>$L56="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="552" priority="560">
+    <cfRule type="expression" dxfId="584" priority="560">
       <formula>$L56="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="551" priority="545">
+    <cfRule type="expression" dxfId="583" priority="545">
       <formula>$L3="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="550" priority="546">
+    <cfRule type="expression" dxfId="582" priority="546">
       <formula>$L3="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="549" priority="547">
+    <cfRule type="expression" dxfId="581" priority="547">
       <formula>$L3="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="548" priority="548">
+    <cfRule type="expression" dxfId="580" priority="548">
       <formula>$L3="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="547" priority="549">
+    <cfRule type="expression" dxfId="579" priority="549">
       <formula>$L3="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="546" priority="550">
+    <cfRule type="expression" dxfId="578" priority="550">
       <formula>$L3="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="545" priority="551">
+    <cfRule type="expression" dxfId="577" priority="551">
       <formula>$L3="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="544" priority="552">
+    <cfRule type="expression" dxfId="576" priority="552">
       <formula>$L3="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="543" priority="537">
+    <cfRule type="expression" dxfId="575" priority="537">
       <formula>$L4="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="542" priority="538">
+    <cfRule type="expression" dxfId="574" priority="538">
       <formula>$L4="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="541" priority="539">
+    <cfRule type="expression" dxfId="573" priority="539">
       <formula>$L4="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="540" priority="540">
+    <cfRule type="expression" dxfId="572" priority="540">
       <formula>$L4="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="539" priority="541">
+    <cfRule type="expression" dxfId="571" priority="541">
       <formula>$L4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="538" priority="542">
+    <cfRule type="expression" dxfId="570" priority="542">
       <formula>$L4="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="537" priority="543">
+    <cfRule type="expression" dxfId="569" priority="543">
       <formula>$L4="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="536" priority="544">
+    <cfRule type="expression" dxfId="568" priority="544">
       <formula>$L4="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C44">
-    <cfRule type="expression" dxfId="535" priority="529">
+    <cfRule type="expression" dxfId="567" priority="529">
       <formula>$L43="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="534" priority="530">
+    <cfRule type="expression" dxfId="566" priority="530">
       <formula>$L43="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="533" priority="531">
+    <cfRule type="expression" dxfId="565" priority="531">
       <formula>$L43="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="532" priority="532">
+    <cfRule type="expression" dxfId="564" priority="532">
       <formula>$L43="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="531" priority="533">
+    <cfRule type="expression" dxfId="563" priority="533">
       <formula>$L43="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="530" priority="534">
+    <cfRule type="expression" dxfId="562" priority="534">
       <formula>$L43="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="529" priority="535">
+    <cfRule type="expression" dxfId="561" priority="535">
       <formula>$L43="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="528" priority="536">
+    <cfRule type="expression" dxfId="560" priority="536">
       <formula>$L43="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="527" priority="425">
+    <cfRule type="expression" dxfId="559" priority="425">
       <formula>$L98="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="526" priority="426">
+    <cfRule type="expression" dxfId="558" priority="426">
       <formula>$L98="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="525" priority="427">
+    <cfRule type="expression" dxfId="557" priority="427">
       <formula>$L98="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="524" priority="428">
+    <cfRule type="expression" dxfId="556" priority="428">
       <formula>$L98="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="523" priority="429">
+    <cfRule type="expression" dxfId="555" priority="429">
       <formula>$L98="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="522" priority="430">
+    <cfRule type="expression" dxfId="554" priority="430">
       <formula>$L98="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="521" priority="431">
+    <cfRule type="expression" dxfId="553" priority="431">
       <formula>$L98="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="520" priority="432">
+    <cfRule type="expression" dxfId="552" priority="432">
       <formula>$L98="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="519" priority="521">
+    <cfRule type="expression" dxfId="551" priority="521">
       <formula>$L70="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="518" priority="522">
+    <cfRule type="expression" dxfId="550" priority="522">
       <formula>$L70="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="517" priority="523">
+    <cfRule type="expression" dxfId="549" priority="523">
       <formula>$L70="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="516" priority="524">
+    <cfRule type="expression" dxfId="548" priority="524">
       <formula>$L70="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="515" priority="525">
+    <cfRule type="expression" dxfId="547" priority="525">
       <formula>$L70="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="514" priority="526">
+    <cfRule type="expression" dxfId="546" priority="526">
       <formula>$L70="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="513" priority="527">
+    <cfRule type="expression" dxfId="545" priority="527">
       <formula>$L70="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="512" priority="528">
+    <cfRule type="expression" dxfId="544" priority="528">
       <formula>$L70="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="511" priority="513">
+    <cfRule type="expression" dxfId="543" priority="513">
       <formula>$L76="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="510" priority="514">
+    <cfRule type="expression" dxfId="542" priority="514">
       <formula>$L76="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="509" priority="515">
+    <cfRule type="expression" dxfId="541" priority="515">
       <formula>$L76="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="508" priority="516">
+    <cfRule type="expression" dxfId="540" priority="516">
       <formula>$L76="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="507" priority="517">
+    <cfRule type="expression" dxfId="539" priority="517">
       <formula>$L76="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="506" priority="518">
+    <cfRule type="expression" dxfId="538" priority="518">
       <formula>$L76="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="505" priority="519">
+    <cfRule type="expression" dxfId="537" priority="519">
       <formula>$L76="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="504" priority="520">
+    <cfRule type="expression" dxfId="536" priority="520">
       <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77:C81">
-    <cfRule type="expression" dxfId="503" priority="505">
+    <cfRule type="expression" dxfId="535" priority="505">
       <formula>$L77="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="502" priority="506">
+    <cfRule type="expression" dxfId="534" priority="506">
       <formula>$L77="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="501" priority="507">
+    <cfRule type="expression" dxfId="533" priority="507">
       <formula>$L77="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="500" priority="508">
+    <cfRule type="expression" dxfId="532" priority="508">
       <formula>$L77="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="499" priority="509">
+    <cfRule type="expression" dxfId="531" priority="509">
       <formula>$L77="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="498" priority="510">
+    <cfRule type="expression" dxfId="530" priority="510">
       <formula>$L77="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="497" priority="511">
+    <cfRule type="expression" dxfId="529" priority="511">
       <formula>$L77="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="496" priority="512">
+    <cfRule type="expression" dxfId="528" priority="512">
       <formula>$L77="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="495" priority="497">
+    <cfRule type="expression" dxfId="527" priority="497">
       <formula>$L82="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="494" priority="498">
+    <cfRule type="expression" dxfId="526" priority="498">
       <formula>$L82="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="493" priority="499">
+    <cfRule type="expression" dxfId="525" priority="499">
       <formula>$L82="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="492" priority="500">
+    <cfRule type="expression" dxfId="524" priority="500">
       <formula>$L82="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="491" priority="501">
+    <cfRule type="expression" dxfId="523" priority="501">
       <formula>$L82="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="490" priority="502">
+    <cfRule type="expression" dxfId="522" priority="502">
       <formula>$L82="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="489" priority="503">
+    <cfRule type="expression" dxfId="521" priority="503">
       <formula>$L82="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="488" priority="504">
+    <cfRule type="expression" dxfId="520" priority="504">
       <formula>$L82="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88">
-    <cfRule type="expression" dxfId="487" priority="489">
+    <cfRule type="expression" dxfId="519" priority="489">
       <formula>$L88="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="486" priority="490">
+    <cfRule type="expression" dxfId="518" priority="490">
       <formula>$L88="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="485" priority="491">
+    <cfRule type="expression" dxfId="517" priority="491">
       <formula>$L88="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="484" priority="492">
+    <cfRule type="expression" dxfId="516" priority="492">
       <formula>$L88="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="483" priority="493">
+    <cfRule type="expression" dxfId="515" priority="493">
       <formula>$L88="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="482" priority="494">
+    <cfRule type="expression" dxfId="514" priority="494">
       <formula>$L88="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="481" priority="495">
+    <cfRule type="expression" dxfId="513" priority="495">
       <formula>$L88="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="480" priority="496">
+    <cfRule type="expression" dxfId="512" priority="496">
       <formula>$L88="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89">
-    <cfRule type="expression" dxfId="479" priority="481">
+    <cfRule type="expression" dxfId="511" priority="481">
       <formula>$L89="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="478" priority="482">
+    <cfRule type="expression" dxfId="510" priority="482">
       <formula>$L89="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="477" priority="483">
+    <cfRule type="expression" dxfId="509" priority="483">
       <formula>$L89="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="476" priority="484">
+    <cfRule type="expression" dxfId="508" priority="484">
       <formula>$L89="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="475" priority="485">
+    <cfRule type="expression" dxfId="507" priority="485">
       <formula>$L89="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="474" priority="486">
+    <cfRule type="expression" dxfId="506" priority="486">
       <formula>$L89="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="473" priority="487">
+    <cfRule type="expression" dxfId="505" priority="487">
       <formula>$L89="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="472" priority="488">
+    <cfRule type="expression" dxfId="504" priority="488">
       <formula>$L89="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="471" priority="473">
+    <cfRule type="expression" dxfId="503" priority="473">
       <formula>$L90="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="470" priority="474">
+    <cfRule type="expression" dxfId="502" priority="474">
       <formula>$L90="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="469" priority="475">
+    <cfRule type="expression" dxfId="501" priority="475">
       <formula>$L90="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="468" priority="476">
+    <cfRule type="expression" dxfId="500" priority="476">
       <formula>$L90="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="467" priority="477">
+    <cfRule type="expression" dxfId="499" priority="477">
       <formula>$L90="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="466" priority="478">
+    <cfRule type="expression" dxfId="498" priority="478">
       <formula>$L90="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="465" priority="479">
+    <cfRule type="expression" dxfId="497" priority="479">
       <formula>$L90="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="464" priority="480">
+    <cfRule type="expression" dxfId="496" priority="480">
       <formula>$L90="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="expression" dxfId="463" priority="465">
+    <cfRule type="expression" dxfId="495" priority="465">
       <formula>$L91="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="462" priority="466">
+    <cfRule type="expression" dxfId="494" priority="466">
       <formula>$L91="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="461" priority="467">
+    <cfRule type="expression" dxfId="493" priority="467">
       <formula>$L91="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="460" priority="468">
+    <cfRule type="expression" dxfId="492" priority="468">
       <formula>$L91="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="459" priority="469">
+    <cfRule type="expression" dxfId="491" priority="469">
       <formula>$L91="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="458" priority="470">
+    <cfRule type="expression" dxfId="490" priority="470">
       <formula>$L91="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="457" priority="471">
+    <cfRule type="expression" dxfId="489" priority="471">
       <formula>$L91="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="456" priority="472">
+    <cfRule type="expression" dxfId="488" priority="472">
       <formula>$L91="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="expression" dxfId="455" priority="457">
+    <cfRule type="expression" dxfId="487" priority="457">
       <formula>$L92="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="454" priority="458">
+    <cfRule type="expression" dxfId="486" priority="458">
       <formula>$L92="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="453" priority="459">
+    <cfRule type="expression" dxfId="485" priority="459">
       <formula>$L92="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="452" priority="460">
+    <cfRule type="expression" dxfId="484" priority="460">
       <formula>$L92="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="451" priority="461">
+    <cfRule type="expression" dxfId="483" priority="461">
       <formula>$L92="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="450" priority="462">
+    <cfRule type="expression" dxfId="482" priority="462">
       <formula>$L92="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="449" priority="463">
+    <cfRule type="expression" dxfId="481" priority="463">
       <formula>$L92="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="448" priority="464">
+    <cfRule type="expression" dxfId="480" priority="464">
       <formula>$L92="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="447" priority="449">
+    <cfRule type="expression" dxfId="479" priority="449">
       <formula>$L93="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="446" priority="450">
+    <cfRule type="expression" dxfId="478" priority="450">
       <formula>$L93="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="445" priority="451">
+    <cfRule type="expression" dxfId="477" priority="451">
       <formula>$L93="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="444" priority="452">
+    <cfRule type="expression" dxfId="476" priority="452">
       <formula>$L93="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="443" priority="453">
+    <cfRule type="expression" dxfId="475" priority="453">
       <formula>$L93="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="442" priority="454">
+    <cfRule type="expression" dxfId="474" priority="454">
       <formula>$L93="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="441" priority="455">
+    <cfRule type="expression" dxfId="473" priority="455">
       <formula>$L93="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="440" priority="456">
+    <cfRule type="expression" dxfId="472" priority="456">
       <formula>$L93="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C96">
-    <cfRule type="expression" dxfId="439" priority="441">
+    <cfRule type="expression" dxfId="471" priority="441">
       <formula>$L94="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="438" priority="442">
+    <cfRule type="expression" dxfId="470" priority="442">
       <formula>$L94="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="437" priority="443">
+    <cfRule type="expression" dxfId="469" priority="443">
       <formula>$L94="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="436" priority="444">
+    <cfRule type="expression" dxfId="468" priority="444">
       <formula>$L94="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="435" priority="445">
+    <cfRule type="expression" dxfId="467" priority="445">
       <formula>$L94="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="434" priority="446">
+    <cfRule type="expression" dxfId="466" priority="446">
       <formula>$L94="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="433" priority="447">
+    <cfRule type="expression" dxfId="465" priority="447">
       <formula>$L94="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="448">
+    <cfRule type="expression" dxfId="464" priority="448">
       <formula>$L94="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="expression" dxfId="431" priority="433">
+    <cfRule type="expression" dxfId="463" priority="433">
       <formula>$L97="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="430" priority="434">
+    <cfRule type="expression" dxfId="462" priority="434">
       <formula>$L97="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="429" priority="435">
+    <cfRule type="expression" dxfId="461" priority="435">
       <formula>$L97="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="428" priority="436">
+    <cfRule type="expression" dxfId="460" priority="436">
       <formula>$L97="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="427" priority="437">
+    <cfRule type="expression" dxfId="459" priority="437">
       <formula>$L97="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="426" priority="438">
+    <cfRule type="expression" dxfId="458" priority="438">
       <formula>$L97="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="425" priority="439">
+    <cfRule type="expression" dxfId="457" priority="439">
       <formula>$L97="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="424" priority="440">
+    <cfRule type="expression" dxfId="456" priority="440">
       <formula>$L97="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C11">
-    <cfRule type="expression" dxfId="423" priority="417">
+    <cfRule type="expression" dxfId="455" priority="417">
       <formula>$L9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="422" priority="418">
+    <cfRule type="expression" dxfId="454" priority="418">
       <formula>$L9="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="421" priority="419">
+    <cfRule type="expression" dxfId="453" priority="419">
       <formula>$L9="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="420">
+    <cfRule type="expression" dxfId="452" priority="420">
       <formula>$L9="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="419" priority="421">
+    <cfRule type="expression" dxfId="451" priority="421">
       <formula>$L9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="418" priority="422">
+    <cfRule type="expression" dxfId="450" priority="422">
       <formula>$L9="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="417" priority="423">
+    <cfRule type="expression" dxfId="449" priority="423">
       <formula>$L9="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="416" priority="424">
+    <cfRule type="expression" dxfId="448" priority="424">
       <formula>$L9="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="415" priority="409">
+    <cfRule type="expression" dxfId="447" priority="409">
       <formula>$L17="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="414" priority="410">
+    <cfRule type="expression" dxfId="446" priority="410">
       <formula>$L17="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="413" priority="411">
+    <cfRule type="expression" dxfId="445" priority="411">
       <formula>$L17="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="412" priority="412">
+    <cfRule type="expression" dxfId="444" priority="412">
       <formula>$L17="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="411" priority="413">
+    <cfRule type="expression" dxfId="443" priority="413">
       <formula>$L17="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="410" priority="414">
+    <cfRule type="expression" dxfId="442" priority="414">
       <formula>$L17="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="409" priority="415">
+    <cfRule type="expression" dxfId="441" priority="415">
       <formula>$L17="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="408" priority="416">
+    <cfRule type="expression" dxfId="440" priority="416">
       <formula>$L17="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="407" priority="401">
+    <cfRule type="expression" dxfId="439" priority="401">
       <formula>$L29="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="406" priority="402">
+    <cfRule type="expression" dxfId="438" priority="402">
       <formula>$L29="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="405" priority="403">
+    <cfRule type="expression" dxfId="437" priority="403">
       <formula>$L29="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="404" priority="404">
+    <cfRule type="expression" dxfId="436" priority="404">
       <formula>$L29="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="403" priority="405">
+    <cfRule type="expression" dxfId="435" priority="405">
       <formula>$L29="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="402" priority="406">
+    <cfRule type="expression" dxfId="434" priority="406">
       <formula>$L29="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="401" priority="407">
+    <cfRule type="expression" dxfId="433" priority="407">
       <formula>$L29="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="400" priority="408">
+    <cfRule type="expression" dxfId="432" priority="408">
       <formula>$L29="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="399" priority="393">
+    <cfRule type="expression" dxfId="431" priority="393">
       <formula>$L33="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="398" priority="394">
+    <cfRule type="expression" dxfId="430" priority="394">
       <formula>$L33="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="397" priority="395">
+    <cfRule type="expression" dxfId="429" priority="395">
       <formula>$L33="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="396" priority="396">
+    <cfRule type="expression" dxfId="428" priority="396">
       <formula>$L33="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="395" priority="397">
+    <cfRule type="expression" dxfId="427" priority="397">
       <formula>$L33="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="394" priority="398">
+    <cfRule type="expression" dxfId="426" priority="398">
       <formula>$L33="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="399">
+    <cfRule type="expression" dxfId="425" priority="399">
       <formula>$L33="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="392" priority="400">
+    <cfRule type="expression" dxfId="424" priority="400">
       <formula>$L33="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="391" priority="377">
+    <cfRule type="expression" dxfId="423" priority="377">
       <formula>$L36="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="378">
+    <cfRule type="expression" dxfId="422" priority="378">
       <formula>$L36="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="389" priority="379">
+    <cfRule type="expression" dxfId="421" priority="379">
       <formula>$L36="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="380">
+    <cfRule type="expression" dxfId="420" priority="380">
       <formula>$L36="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="381">
+    <cfRule type="expression" dxfId="419" priority="381">
       <formula>$L36="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="386" priority="382">
+    <cfRule type="expression" dxfId="418" priority="382">
       <formula>$L36="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="385" priority="383">
+    <cfRule type="expression" dxfId="417" priority="383">
       <formula>$L36="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="384" priority="384">
+    <cfRule type="expression" dxfId="416" priority="384">
       <formula>$L36="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="383" priority="385">
+    <cfRule type="expression" dxfId="415" priority="385">
       <formula>$L35="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="386">
+    <cfRule type="expression" dxfId="414" priority="386">
       <formula>$L35="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="381" priority="387">
+    <cfRule type="expression" dxfId="413" priority="387">
       <formula>$L35="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="380" priority="388">
+    <cfRule type="expression" dxfId="412" priority="388">
       <formula>$L35="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="379" priority="389">
+    <cfRule type="expression" dxfId="411" priority="389">
       <formula>$L35="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="378" priority="390">
+    <cfRule type="expression" dxfId="410" priority="390">
       <formula>$L35="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="377" priority="391">
+    <cfRule type="expression" dxfId="409" priority="391">
       <formula>$L35="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="376" priority="392">
+    <cfRule type="expression" dxfId="408" priority="392">
       <formula>$L35="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="375" priority="369">
+    <cfRule type="expression" dxfId="407" priority="369">
       <formula>$L56="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="374" priority="370">
+    <cfRule type="expression" dxfId="406" priority="370">
       <formula>$L56="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="373" priority="371">
+    <cfRule type="expression" dxfId="405" priority="371">
       <formula>$L56="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="372" priority="372">
+    <cfRule type="expression" dxfId="404" priority="372">
       <formula>$L56="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="373">
+    <cfRule type="expression" dxfId="403" priority="373">
       <formula>$L56="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="370" priority="374">
+    <cfRule type="expression" dxfId="402" priority="374">
       <formula>$L56="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="369" priority="375">
+    <cfRule type="expression" dxfId="401" priority="375">
       <formula>$L56="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="376">
+    <cfRule type="expression" dxfId="400" priority="376">
       <formula>$L56="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="367" priority="361">
+    <cfRule type="expression" dxfId="399" priority="361">
       <formula>$L3="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="366" priority="362">
+    <cfRule type="expression" dxfId="398" priority="362">
       <formula>$L3="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="365" priority="363">
+    <cfRule type="expression" dxfId="397" priority="363">
       <formula>$L3="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="364">
+    <cfRule type="expression" dxfId="396" priority="364">
       <formula>$L3="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="363" priority="365">
+    <cfRule type="expression" dxfId="395" priority="365">
       <formula>$L3="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="366">
+    <cfRule type="expression" dxfId="394" priority="366">
       <formula>$L3="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="361" priority="367">
+    <cfRule type="expression" dxfId="393" priority="367">
       <formula>$L3="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="360" priority="368">
+    <cfRule type="expression" dxfId="392" priority="368">
       <formula>$L3="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="359" priority="353">
+    <cfRule type="expression" dxfId="391" priority="353">
       <formula>$L4="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="358" priority="354">
+    <cfRule type="expression" dxfId="390" priority="354">
       <formula>$L4="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="357" priority="355">
+    <cfRule type="expression" dxfId="389" priority="355">
       <formula>$L4="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="356">
+    <cfRule type="expression" dxfId="388" priority="356">
       <formula>$L4="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="355" priority="357">
+    <cfRule type="expression" dxfId="387" priority="357">
       <formula>$L4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="354" priority="358">
+    <cfRule type="expression" dxfId="386" priority="358">
       <formula>$L4="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="353" priority="359">
+    <cfRule type="expression" dxfId="385" priority="359">
       <formula>$L4="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="352" priority="360">
+    <cfRule type="expression" dxfId="384" priority="360">
       <formula>$L4="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="expression" dxfId="351" priority="345">
+    <cfRule type="expression" dxfId="383" priority="345">
       <formula>$L43="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="346">
+    <cfRule type="expression" dxfId="382" priority="346">
       <formula>$L43="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="349" priority="347">
+    <cfRule type="expression" dxfId="381" priority="347">
       <formula>$L43="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="348" priority="348">
+    <cfRule type="expression" dxfId="380" priority="348">
       <formula>$L43="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="349">
+    <cfRule type="expression" dxfId="379" priority="349">
       <formula>$L43="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="350">
+    <cfRule type="expression" dxfId="378" priority="350">
       <formula>$L43="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="345" priority="351">
+    <cfRule type="expression" dxfId="377" priority="351">
       <formula>$L43="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="352">
+    <cfRule type="expression" dxfId="376" priority="352">
       <formula>$L43="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="expression" dxfId="343" priority="241">
+    <cfRule type="expression" dxfId="375" priority="241">
       <formula>$L98="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="242">
+    <cfRule type="expression" dxfId="374" priority="242">
       <formula>$L98="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="243">
+    <cfRule type="expression" dxfId="373" priority="243">
       <formula>$L98="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="340" priority="244">
+    <cfRule type="expression" dxfId="372" priority="244">
       <formula>$L98="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="339" priority="245">
+    <cfRule type="expression" dxfId="371" priority="245">
       <formula>$L98="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="246">
+    <cfRule type="expression" dxfId="370" priority="246">
       <formula>$L98="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="337" priority="247">
+    <cfRule type="expression" dxfId="369" priority="247">
       <formula>$L98="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="336" priority="248">
+    <cfRule type="expression" dxfId="368" priority="248">
       <formula>$L98="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="expression" dxfId="335" priority="337">
+    <cfRule type="expression" dxfId="367" priority="337">
       <formula>$L70="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="338">
+    <cfRule type="expression" dxfId="366" priority="338">
       <formula>$L70="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="333" priority="339">
+    <cfRule type="expression" dxfId="365" priority="339">
       <formula>$L70="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="340">
+    <cfRule type="expression" dxfId="364" priority="340">
       <formula>$L70="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="341">
+    <cfRule type="expression" dxfId="363" priority="341">
       <formula>$L70="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="342">
+    <cfRule type="expression" dxfId="362" priority="342">
       <formula>$L70="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="343">
+    <cfRule type="expression" dxfId="361" priority="343">
       <formula>$L70="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="344">
+    <cfRule type="expression" dxfId="360" priority="344">
       <formula>$L70="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="expression" dxfId="327" priority="329">
+    <cfRule type="expression" dxfId="359" priority="329">
       <formula>$L76="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="330">
+    <cfRule type="expression" dxfId="358" priority="330">
       <formula>$L76="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="325" priority="331">
+    <cfRule type="expression" dxfId="357" priority="331">
       <formula>$L76="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="332">
+    <cfRule type="expression" dxfId="356" priority="332">
       <formula>$L76="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="333">
+    <cfRule type="expression" dxfId="355" priority="333">
       <formula>$L76="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="334">
+    <cfRule type="expression" dxfId="354" priority="334">
       <formula>$L76="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="321" priority="335">
+    <cfRule type="expression" dxfId="353" priority="335">
       <formula>$L76="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="336">
+    <cfRule type="expression" dxfId="352" priority="336">
       <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77:D81">
-    <cfRule type="expression" dxfId="319" priority="321">
+    <cfRule type="expression" dxfId="351" priority="321">
       <formula>$L77="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="318" priority="322">
+    <cfRule type="expression" dxfId="350" priority="322">
       <formula>$L77="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="323">
+    <cfRule type="expression" dxfId="349" priority="323">
       <formula>$L77="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="316" priority="324">
+    <cfRule type="expression" dxfId="348" priority="324">
       <formula>$L77="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="315" priority="325">
+    <cfRule type="expression" dxfId="347" priority="325">
       <formula>$L77="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="326">
+    <cfRule type="expression" dxfId="346" priority="326">
       <formula>$L77="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="313" priority="327">
+    <cfRule type="expression" dxfId="345" priority="327">
       <formula>$L77="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="312" priority="328">
+    <cfRule type="expression" dxfId="344" priority="328">
       <formula>$L77="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D82:D87">
-    <cfRule type="expression" dxfId="311" priority="313">
+    <cfRule type="expression" dxfId="343" priority="313">
       <formula>$L82="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="310" priority="314">
+    <cfRule type="expression" dxfId="342" priority="314">
       <formula>$L82="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="309" priority="315">
+    <cfRule type="expression" dxfId="341" priority="315">
       <formula>$L82="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="316">
+    <cfRule type="expression" dxfId="340" priority="316">
       <formula>$L82="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="307" priority="317">
+    <cfRule type="expression" dxfId="339" priority="317">
       <formula>$L82="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="318">
+    <cfRule type="expression" dxfId="338" priority="318">
       <formula>$L82="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="305" priority="319">
+    <cfRule type="expression" dxfId="337" priority="319">
       <formula>$L82="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="320">
+    <cfRule type="expression" dxfId="336" priority="320">
       <formula>$L82="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="expression" dxfId="303" priority="305">
+    <cfRule type="expression" dxfId="335" priority="305">
       <formula>$L88="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="306">
+    <cfRule type="expression" dxfId="334" priority="306">
       <formula>$L88="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="307">
+    <cfRule type="expression" dxfId="333" priority="307">
       <formula>$L88="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="308">
+    <cfRule type="expression" dxfId="332" priority="308">
       <formula>$L88="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="309">
+    <cfRule type="expression" dxfId="331" priority="309">
       <formula>$L88="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="310">
+    <cfRule type="expression" dxfId="330" priority="310">
       <formula>$L88="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="311">
+    <cfRule type="expression" dxfId="329" priority="311">
       <formula>$L88="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="296" priority="312">
+    <cfRule type="expression" dxfId="328" priority="312">
       <formula>$L88="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="295" priority="297">
+    <cfRule type="expression" dxfId="327" priority="297">
       <formula>$L89="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="298">
+    <cfRule type="expression" dxfId="326" priority="298">
       <formula>$L89="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="299">
+    <cfRule type="expression" dxfId="325" priority="299">
       <formula>$L89="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="300">
+    <cfRule type="expression" dxfId="324" priority="300">
       <formula>$L89="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="301">
+    <cfRule type="expression" dxfId="323" priority="301">
       <formula>$L89="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="302">
+    <cfRule type="expression" dxfId="322" priority="302">
       <formula>$L89="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="303">
+    <cfRule type="expression" dxfId="321" priority="303">
       <formula>$L89="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="304">
+    <cfRule type="expression" dxfId="320" priority="304">
       <formula>$L89="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D90">
-    <cfRule type="expression" dxfId="287" priority="289">
+    <cfRule type="expression" dxfId="319" priority="289">
       <formula>$L90="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="290">
+    <cfRule type="expression" dxfId="318" priority="290">
       <formula>$L90="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="291">
+    <cfRule type="expression" dxfId="317" priority="291">
       <formula>$L90="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="292">
+    <cfRule type="expression" dxfId="316" priority="292">
       <formula>$L90="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="293">
+    <cfRule type="expression" dxfId="315" priority="293">
       <formula>$L90="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="294">
+    <cfRule type="expression" dxfId="314" priority="294">
       <formula>$L90="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="295">
+    <cfRule type="expression" dxfId="313" priority="295">
       <formula>$L90="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="296">
+    <cfRule type="expression" dxfId="312" priority="296">
       <formula>$L90="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="expression" dxfId="279" priority="281">
+    <cfRule type="expression" dxfId="311" priority="281">
       <formula>$L91="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="282">
+    <cfRule type="expression" dxfId="310" priority="282">
       <formula>$L91="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="283">
+    <cfRule type="expression" dxfId="309" priority="283">
       <formula>$L91="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="284">
+    <cfRule type="expression" dxfId="308" priority="284">
       <formula>$L91="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="285">
+    <cfRule type="expression" dxfId="307" priority="285">
       <formula>$L91="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="286">
+    <cfRule type="expression" dxfId="306" priority="286">
       <formula>$L91="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="287">
+    <cfRule type="expression" dxfId="305" priority="287">
       <formula>$L91="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="288">
+    <cfRule type="expression" dxfId="304" priority="288">
       <formula>$L91="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="expression" dxfId="271" priority="273">
+    <cfRule type="expression" dxfId="303" priority="273">
       <formula>$L92="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="274">
+    <cfRule type="expression" dxfId="302" priority="274">
       <formula>$L92="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="275">
+    <cfRule type="expression" dxfId="301" priority="275">
       <formula>$L92="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="276">
+    <cfRule type="expression" dxfId="300" priority="276">
       <formula>$L92="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="277">
+    <cfRule type="expression" dxfId="299" priority="277">
       <formula>$L92="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="278">
+    <cfRule type="expression" dxfId="298" priority="278">
       <formula>$L92="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="279">
+    <cfRule type="expression" dxfId="297" priority="279">
       <formula>$L92="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="280">
+    <cfRule type="expression" dxfId="296" priority="280">
       <formula>$L92="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="expression" dxfId="263" priority="265">
+    <cfRule type="expression" dxfId="295" priority="265">
       <formula>$L93="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="266">
+    <cfRule type="expression" dxfId="294" priority="266">
       <formula>$L93="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="267">
+    <cfRule type="expression" dxfId="293" priority="267">
       <formula>$L93="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="268">
+    <cfRule type="expression" dxfId="292" priority="268">
       <formula>$L93="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="269">
+    <cfRule type="expression" dxfId="291" priority="269">
       <formula>$L93="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="270">
+    <cfRule type="expression" dxfId="290" priority="270">
       <formula>$L93="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="271">
+    <cfRule type="expression" dxfId="289" priority="271">
       <formula>$L93="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="272">
+    <cfRule type="expression" dxfId="288" priority="272">
       <formula>$L93="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94:D96">
-    <cfRule type="expression" dxfId="255" priority="257">
+    <cfRule type="expression" dxfId="287" priority="257">
       <formula>$L94="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="258">
+    <cfRule type="expression" dxfId="286" priority="258">
       <formula>$L94="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="259">
+    <cfRule type="expression" dxfId="285" priority="259">
       <formula>$L94="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="260">
+    <cfRule type="expression" dxfId="284" priority="260">
       <formula>$L94="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="261">
+    <cfRule type="expression" dxfId="283" priority="261">
       <formula>$L94="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="262">
+    <cfRule type="expression" dxfId="282" priority="262">
       <formula>$L94="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="263">
+    <cfRule type="expression" dxfId="281" priority="263">
       <formula>$L94="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="264">
+    <cfRule type="expression" dxfId="280" priority="264">
       <formula>$L94="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97">
-    <cfRule type="expression" dxfId="247" priority="249">
+    <cfRule type="expression" dxfId="279" priority="249">
       <formula>$L97="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="250">
+    <cfRule type="expression" dxfId="278" priority="250">
       <formula>$L97="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="251">
+    <cfRule type="expression" dxfId="277" priority="251">
       <formula>$L97="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="252">
+    <cfRule type="expression" dxfId="276" priority="252">
       <formula>$L97="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="253">
+    <cfRule type="expression" dxfId="275" priority="253">
       <formula>$L97="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="254">
+    <cfRule type="expression" dxfId="274" priority="254">
       <formula>$L97="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="255">
+    <cfRule type="expression" dxfId="273" priority="255">
       <formula>$L97="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="256">
+    <cfRule type="expression" dxfId="272" priority="256">
       <formula>$L97="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D11">
-    <cfRule type="expression" dxfId="239" priority="233">
+    <cfRule type="expression" dxfId="271" priority="233">
       <formula>$L9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="234">
+    <cfRule type="expression" dxfId="270" priority="234">
       <formula>$L9="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="235">
+    <cfRule type="expression" dxfId="269" priority="235">
       <formula>$L9="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="236">
+    <cfRule type="expression" dxfId="268" priority="236">
       <formula>$L9="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="237">
+    <cfRule type="expression" dxfId="267" priority="237">
       <formula>$L9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="238">
+    <cfRule type="expression" dxfId="266" priority="238">
       <formula>$L9="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="239">
+    <cfRule type="expression" dxfId="265" priority="239">
       <formula>$L9="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="240">
+    <cfRule type="expression" dxfId="264" priority="240">
       <formula>$L9="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="231" priority="225">
+    <cfRule type="expression" dxfId="263" priority="225">
       <formula>$L17="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="226">
+    <cfRule type="expression" dxfId="262" priority="226">
       <formula>$L17="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="227">
+    <cfRule type="expression" dxfId="261" priority="227">
       <formula>$L17="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="228">
+    <cfRule type="expression" dxfId="260" priority="228">
       <formula>$L17="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="229">
+    <cfRule type="expression" dxfId="259" priority="229">
       <formula>$L17="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="230">
+    <cfRule type="expression" dxfId="258" priority="230">
       <formula>$L17="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="231">
+    <cfRule type="expression" dxfId="257" priority="231">
       <formula>$L17="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="232">
+    <cfRule type="expression" dxfId="256" priority="232">
       <formula>$L17="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="expression" dxfId="223" priority="217">
+    <cfRule type="expression" dxfId="255" priority="217">
       <formula>$L29="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="218">
+    <cfRule type="expression" dxfId="254" priority="218">
       <formula>$L29="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="219">
+    <cfRule type="expression" dxfId="253" priority="219">
       <formula>$L29="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="220">
+    <cfRule type="expression" dxfId="252" priority="220">
       <formula>$L29="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="221">
+    <cfRule type="expression" dxfId="251" priority="221">
       <formula>$L29="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="222">
+    <cfRule type="expression" dxfId="250" priority="222">
       <formula>$L29="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="223">
+    <cfRule type="expression" dxfId="249" priority="223">
       <formula>$L29="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="224">
+    <cfRule type="expression" dxfId="248" priority="224">
       <formula>$L29="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="expression" dxfId="215" priority="209">
+    <cfRule type="expression" dxfId="247" priority="209">
       <formula>$L33="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="210">
+    <cfRule type="expression" dxfId="246" priority="210">
       <formula>$L33="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="211">
+    <cfRule type="expression" dxfId="245" priority="211">
       <formula>$L33="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="212">
+    <cfRule type="expression" dxfId="244" priority="212">
       <formula>$L33="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="213">
+    <cfRule type="expression" dxfId="243" priority="213">
       <formula>$L33="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="214">
+    <cfRule type="expression" dxfId="242" priority="214">
       <formula>$L33="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="215">
+    <cfRule type="expression" dxfId="241" priority="215">
       <formula>$L33="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="216">
+    <cfRule type="expression" dxfId="240" priority="216">
       <formula>$L33="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="207" priority="193">
+    <cfRule type="expression" dxfId="239" priority="193">
       <formula>$L36="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="194">
+    <cfRule type="expression" dxfId="238" priority="194">
       <formula>$L36="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="195">
+    <cfRule type="expression" dxfId="237" priority="195">
       <formula>$L36="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="196">
+    <cfRule type="expression" dxfId="236" priority="196">
       <formula>$L36="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="197">
+    <cfRule type="expression" dxfId="235" priority="197">
       <formula>$L36="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="198">
+    <cfRule type="expression" dxfId="234" priority="198">
       <formula>$L36="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="199">
+    <cfRule type="expression" dxfId="233" priority="199">
       <formula>$L36="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="200">
+    <cfRule type="expression" dxfId="232" priority="200">
       <formula>$L36="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="199" priority="201">
+    <cfRule type="expression" dxfId="231" priority="201">
       <formula>$L35="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="202">
+    <cfRule type="expression" dxfId="230" priority="202">
       <formula>$L35="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="203">
+    <cfRule type="expression" dxfId="229" priority="203">
       <formula>$L35="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="204">
+    <cfRule type="expression" dxfId="228" priority="204">
       <formula>$L35="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="205">
+    <cfRule type="expression" dxfId="227" priority="205">
       <formula>$L35="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="206">
+    <cfRule type="expression" dxfId="226" priority="206">
       <formula>$L35="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="207">
+    <cfRule type="expression" dxfId="225" priority="207">
       <formula>$L35="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="208">
+    <cfRule type="expression" dxfId="224" priority="208">
       <formula>$L35="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="expression" dxfId="191" priority="185">
+    <cfRule type="expression" dxfId="223" priority="185">
       <formula>$L56="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="186">
+    <cfRule type="expression" dxfId="222" priority="186">
       <formula>$L56="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="187">
+    <cfRule type="expression" dxfId="221" priority="187">
       <formula>$L56="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="188">
+    <cfRule type="expression" dxfId="220" priority="188">
       <formula>$L56="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="189">
+    <cfRule type="expression" dxfId="219" priority="189">
       <formula>$L56="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="190">
+    <cfRule type="expression" dxfId="218" priority="190">
       <formula>$L56="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="191">
+    <cfRule type="expression" dxfId="217" priority="191">
       <formula>$L56="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="192">
+    <cfRule type="expression" dxfId="216" priority="192">
       <formula>$L56="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="183" priority="177">
+    <cfRule type="expression" dxfId="215" priority="177">
       <formula>$L3="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="178">
+    <cfRule type="expression" dxfId="214" priority="178">
       <formula>$L3="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="179">
+    <cfRule type="expression" dxfId="213" priority="179">
       <formula>$L3="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="180">
+    <cfRule type="expression" dxfId="212" priority="180">
       <formula>$L3="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="181">
+    <cfRule type="expression" dxfId="211" priority="181">
       <formula>$L3="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="182">
+    <cfRule type="expression" dxfId="210" priority="182">
       <formula>$L3="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="183">
+    <cfRule type="expression" dxfId="209" priority="183">
       <formula>$L3="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="184">
+    <cfRule type="expression" dxfId="208" priority="184">
       <formula>$L3="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="175" priority="169">
+    <cfRule type="expression" dxfId="207" priority="169">
       <formula>$L4="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="170">
+    <cfRule type="expression" dxfId="206" priority="170">
       <formula>$L4="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="171">
+    <cfRule type="expression" dxfId="205" priority="171">
       <formula>$L4="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="172">
+    <cfRule type="expression" dxfId="204" priority="172">
       <formula>$L4="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="173">
+    <cfRule type="expression" dxfId="203" priority="173">
       <formula>$L4="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="174">
+    <cfRule type="expression" dxfId="202" priority="174">
       <formula>$L4="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="175">
+    <cfRule type="expression" dxfId="201" priority="175">
       <formula>$L4="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="176">
+    <cfRule type="expression" dxfId="200" priority="176">
       <formula>$L4="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:E44">
-    <cfRule type="expression" dxfId="167" priority="161">
+    <cfRule type="expression" dxfId="199" priority="161">
       <formula>$L43="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="162">
+    <cfRule type="expression" dxfId="198" priority="162">
       <formula>$L43="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="163">
+    <cfRule type="expression" dxfId="197" priority="163">
       <formula>$L43="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="164">
+    <cfRule type="expression" dxfId="196" priority="164">
       <formula>$L43="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="165">
+    <cfRule type="expression" dxfId="195" priority="165">
       <formula>$L43="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="166">
+    <cfRule type="expression" dxfId="194" priority="166">
       <formula>$L43="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="167">
+    <cfRule type="expression" dxfId="193" priority="167">
       <formula>$L43="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="168">
+    <cfRule type="expression" dxfId="192" priority="168">
       <formula>$L43="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98">
-    <cfRule type="expression" dxfId="159" priority="57">
+    <cfRule type="expression" dxfId="191" priority="57">
       <formula>$L98="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="58">
+    <cfRule type="expression" dxfId="190" priority="58">
       <formula>$L98="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="59">
+    <cfRule type="expression" dxfId="189" priority="59">
       <formula>$L98="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="60">
+    <cfRule type="expression" dxfId="188" priority="60">
       <formula>$L98="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="61">
+    <cfRule type="expression" dxfId="187" priority="61">
       <formula>$L98="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="62">
+    <cfRule type="expression" dxfId="186" priority="62">
       <formula>$L98="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="63">
+    <cfRule type="expression" dxfId="185" priority="63">
       <formula>$L98="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="64">
+    <cfRule type="expression" dxfId="184" priority="64">
       <formula>$L98="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="expression" dxfId="151" priority="153">
+    <cfRule type="expression" dxfId="183" priority="153">
       <formula>$L70="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="154">
+    <cfRule type="expression" dxfId="182" priority="154">
       <formula>$L70="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="155">
+    <cfRule type="expression" dxfId="181" priority="155">
       <formula>$L70="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="156">
+    <cfRule type="expression" dxfId="180" priority="156">
       <formula>$L70="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="157">
+    <cfRule type="expression" dxfId="179" priority="157">
       <formula>$L70="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="158">
+    <cfRule type="expression" dxfId="178" priority="158">
       <formula>$L70="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="159">
+    <cfRule type="expression" dxfId="177" priority="159">
       <formula>$L70="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="160">
+    <cfRule type="expression" dxfId="176" priority="160">
       <formula>$L70="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="expression" dxfId="143" priority="145">
+    <cfRule type="expression" dxfId="175" priority="145">
       <formula>$L76="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="146">
+    <cfRule type="expression" dxfId="174" priority="146">
       <formula>$L76="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="147">
+    <cfRule type="expression" dxfId="173" priority="147">
       <formula>$L76="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="148">
+    <cfRule type="expression" dxfId="172" priority="148">
       <formula>$L76="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="149">
+    <cfRule type="expression" dxfId="171" priority="149">
       <formula>$L76="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="150">
+    <cfRule type="expression" dxfId="170" priority="150">
       <formula>$L76="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="151">
+    <cfRule type="expression" dxfId="169" priority="151">
       <formula>$L76="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="152">
+    <cfRule type="expression" dxfId="168" priority="152">
       <formula>$L76="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77:E81">
-    <cfRule type="expression" dxfId="135" priority="137">
+    <cfRule type="expression" dxfId="167" priority="137">
       <formula>$L77="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="138">
+    <cfRule type="expression" dxfId="166" priority="138">
       <formula>$L77="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="139">
+    <cfRule type="expression" dxfId="165" priority="139">
       <formula>$L77="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="140">
+    <cfRule type="expression" dxfId="164" priority="140">
       <formula>$L77="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="141">
+    <cfRule type="expression" dxfId="163" priority="141">
       <formula>$L77="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="142">
+    <cfRule type="expression" dxfId="162" priority="142">
       <formula>$L77="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="143">
+    <cfRule type="expression" dxfId="161" priority="143">
       <formula>$L77="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="144">
+    <cfRule type="expression" dxfId="160" priority="144">
       <formula>$L77="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82:E87">
-    <cfRule type="expression" dxfId="127" priority="129">
+    <cfRule type="expression" dxfId="159" priority="129">
       <formula>$L82="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="130">
+    <cfRule type="expression" dxfId="158" priority="130">
       <formula>$L82="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="131">
+    <cfRule type="expression" dxfId="157" priority="131">
       <formula>$L82="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="132">
+    <cfRule type="expression" dxfId="156" priority="132">
       <formula>$L82="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="133">
+    <cfRule type="expression" dxfId="155" priority="133">
       <formula>$L82="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="134">
+    <cfRule type="expression" dxfId="154" priority="134">
       <formula>$L82="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="135">
+    <cfRule type="expression" dxfId="153" priority="135">
       <formula>$L82="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="136">
+    <cfRule type="expression" dxfId="152" priority="136">
       <formula>$L82="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E88">
-    <cfRule type="expression" dxfId="119" priority="121">
+    <cfRule type="expression" dxfId="151" priority="121">
       <formula>$L88="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="122">
+    <cfRule type="expression" dxfId="150" priority="122">
       <formula>$L88="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="123">
+    <cfRule type="expression" dxfId="149" priority="123">
       <formula>$L88="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="124">
+    <cfRule type="expression" dxfId="148" priority="124">
       <formula>$L88="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="125">
+    <cfRule type="expression" dxfId="147" priority="125">
       <formula>$L88="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="126">
+    <cfRule type="expression" dxfId="146" priority="126">
       <formula>$L88="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="127">
+    <cfRule type="expression" dxfId="145" priority="127">
       <formula>$L88="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="128">
+    <cfRule type="expression" dxfId="144" priority="128">
       <formula>$L88="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E89">
-    <cfRule type="expression" dxfId="111" priority="113">
+    <cfRule type="expression" dxfId="143" priority="113">
       <formula>$L89="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="114">
+    <cfRule type="expression" dxfId="142" priority="114">
       <formula>$L89="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="115">
+    <cfRule type="expression" dxfId="141" priority="115">
       <formula>$L89="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="116">
+    <cfRule type="expression" dxfId="140" priority="116">
       <formula>$L89="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="117">
+    <cfRule type="expression" dxfId="139" priority="117">
       <formula>$L89="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="118">
+    <cfRule type="expression" dxfId="138" priority="118">
       <formula>$L89="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="119">
+    <cfRule type="expression" dxfId="137" priority="119">
       <formula>$L89="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="120">
+    <cfRule type="expression" dxfId="136" priority="120">
       <formula>$L89="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="expression" dxfId="103" priority="105">
+    <cfRule type="expression" dxfId="135" priority="105">
       <formula>$L90="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="106">
+    <cfRule type="expression" dxfId="134" priority="106">
       <formula>$L90="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="107">
+    <cfRule type="expression" dxfId="133" priority="107">
       <formula>$L90="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="108">
+    <cfRule type="expression" dxfId="132" priority="108">
       <formula>$L90="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="109">
+    <cfRule type="expression" dxfId="131" priority="109">
       <formula>$L90="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="110">
+    <cfRule type="expression" dxfId="130" priority="110">
       <formula>$L90="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="111">
+    <cfRule type="expression" dxfId="129" priority="111">
       <formula>$L90="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="112">
+    <cfRule type="expression" dxfId="128" priority="112">
       <formula>$L90="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="expression" dxfId="95" priority="97">
+    <cfRule type="expression" dxfId="127" priority="97">
       <formula>$L91="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="98">
+    <cfRule type="expression" dxfId="126" priority="98">
       <formula>$L91="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="99">
+    <cfRule type="expression" dxfId="125" priority="99">
       <formula>$L91="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="100">
+    <cfRule type="expression" dxfId="124" priority="100">
       <formula>$L91="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="101">
+    <cfRule type="expression" dxfId="123" priority="101">
       <formula>$L91="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="102">
+    <cfRule type="expression" dxfId="122" priority="102">
       <formula>$L91="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="103">
+    <cfRule type="expression" dxfId="121" priority="103">
       <formula>$L91="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="104">
+    <cfRule type="expression" dxfId="120" priority="104">
       <formula>$L91="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="expression" dxfId="87" priority="89">
+    <cfRule type="expression" dxfId="119" priority="89">
       <formula>$L92="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="90">
+    <cfRule type="expression" dxfId="118" priority="90">
       <formula>$L92="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="91">
+    <cfRule type="expression" dxfId="117" priority="91">
       <formula>$L92="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="92">
+    <cfRule type="expression" dxfId="116" priority="92">
       <formula>$L92="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="93">
+    <cfRule type="expression" dxfId="115" priority="93">
       <formula>$L92="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="94">
+    <cfRule type="expression" dxfId="114" priority="94">
       <formula>$L92="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="95">
+    <cfRule type="expression" dxfId="113" priority="95">
       <formula>$L92="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="96">
+    <cfRule type="expression" dxfId="112" priority="96">
       <formula>$L92="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="expression" dxfId="79" priority="81">
+    <cfRule type="expression" dxfId="111" priority="81">
       <formula>$L93="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="82">
+    <cfRule type="expression" dxfId="110" priority="82">
       <formula>$L93="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="83">
+    <cfRule type="expression" dxfId="109" priority="83">
       <formula>$L93="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="84">
+    <cfRule type="expression" dxfId="108" priority="84">
       <formula>$L93="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="85">
+    <cfRule type="expression" dxfId="107" priority="85">
       <formula>$L93="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="86">
+    <cfRule type="expression" dxfId="106" priority="86">
       <formula>$L93="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="87">
+    <cfRule type="expression" dxfId="105" priority="87">
       <formula>$L93="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88">
+    <cfRule type="expression" dxfId="104" priority="88">
       <formula>$L93="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94:E96">
-    <cfRule type="expression" dxfId="71" priority="73">
+    <cfRule type="expression" dxfId="103" priority="73">
       <formula>$L94="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="74">
+    <cfRule type="expression" dxfId="102" priority="74">
       <formula>$L94="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="75">
+    <cfRule type="expression" dxfId="101" priority="75">
       <formula>$L94="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="76">
+    <cfRule type="expression" dxfId="100" priority="76">
       <formula>$L94="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="77">
+    <cfRule type="expression" dxfId="99" priority="77">
       <formula>$L94="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="78">
+    <cfRule type="expression" dxfId="98" priority="78">
       <formula>$L94="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="79">
+    <cfRule type="expression" dxfId="97" priority="79">
       <formula>$L94="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="80">
+    <cfRule type="expression" dxfId="96" priority="80">
       <formula>$L94="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="expression" dxfId="63" priority="65">
+    <cfRule type="expression" dxfId="95" priority="65">
       <formula>$L97="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="66">
+    <cfRule type="expression" dxfId="94" priority="66">
       <formula>$L97="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="67">
+    <cfRule type="expression" dxfId="93" priority="67">
       <formula>$L97="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="68">
+    <cfRule type="expression" dxfId="92" priority="68">
       <formula>$L97="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="69">
+    <cfRule type="expression" dxfId="91" priority="69">
       <formula>$L97="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="70">
+    <cfRule type="expression" dxfId="90" priority="70">
       <formula>$L97="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="71">
+    <cfRule type="expression" dxfId="89" priority="71">
       <formula>$L97="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="72">
+    <cfRule type="expression" dxfId="88" priority="72">
       <formula>$L97="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="expression" dxfId="55" priority="49">
+    <cfRule type="expression" dxfId="87" priority="49">
       <formula>$L9="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="50">
+    <cfRule type="expression" dxfId="86" priority="50">
       <formula>$L9="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="51">
+    <cfRule type="expression" dxfId="85" priority="51">
       <formula>$L9="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="52">
+    <cfRule type="expression" dxfId="84" priority="52">
       <formula>$L9="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="83" priority="53">
       <formula>$L9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="54">
+    <cfRule type="expression" dxfId="82" priority="54">
       <formula>$L9="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="55">
+    <cfRule type="expression" dxfId="81" priority="55">
       <formula>$L9="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="56">
+    <cfRule type="expression" dxfId="80" priority="56">
       <formula>$L9="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="47" priority="41">
+    <cfRule type="expression" dxfId="79" priority="41">
       <formula>$L17="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42">
+    <cfRule type="expression" dxfId="78" priority="42">
       <formula>$L17="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="43">
+    <cfRule type="expression" dxfId="77" priority="43">
       <formula>$L17="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="44">
+    <cfRule type="expression" dxfId="76" priority="44">
       <formula>$L17="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45">
+    <cfRule type="expression" dxfId="75" priority="45">
       <formula>$L17="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="46">
+    <cfRule type="expression" dxfId="74" priority="46">
       <formula>$L17="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="47">
+    <cfRule type="expression" dxfId="73" priority="47">
       <formula>$L17="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="48">
+    <cfRule type="expression" dxfId="72" priority="48">
       <formula>$L17="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="71" priority="33">
       <formula>$L29="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="70" priority="34">
       <formula>$L29="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
+    <cfRule type="expression" dxfId="69" priority="35">
       <formula>$L29="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
+    <cfRule type="expression" dxfId="68" priority="36">
       <formula>$L29="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
+    <cfRule type="expression" dxfId="67" priority="37">
       <formula>$L29="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
+    <cfRule type="expression" dxfId="66" priority="38">
       <formula>$L29="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="65" priority="39">
       <formula>$L29="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
+    <cfRule type="expression" dxfId="64" priority="40">
       <formula>$L29="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="63" priority="25">
       <formula>$L33="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="62" priority="26">
       <formula>$L33="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
+    <cfRule type="expression" dxfId="61" priority="27">
       <formula>$L33="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
+    <cfRule type="expression" dxfId="60" priority="28">
       <formula>$L33="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="59" priority="29">
       <formula>$L33="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="58" priority="30">
       <formula>$L33="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
+    <cfRule type="expression" dxfId="57" priority="31">
       <formula>$L33="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
+    <cfRule type="expression" dxfId="56" priority="32">
       <formula>$L33="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" dxfId="23" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>$L36="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="54" priority="10">
       <formula>$L36="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="11">
+    <cfRule type="expression" dxfId="53" priority="11">
       <formula>$L36="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="52" priority="12">
       <formula>$L36="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="51" priority="13">
       <formula>$L36="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="50" priority="14">
       <formula>$L36="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="49" priority="15">
       <formula>$L36="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
+    <cfRule type="expression" dxfId="48" priority="16">
       <formula>$L36="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="47" priority="17">
       <formula>$L35="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="46" priority="18">
       <formula>$L35="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="19">
+    <cfRule type="expression" dxfId="45" priority="19">
       <formula>$L35="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="44" priority="20">
       <formula>$L35="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>$L35="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>$L35="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>$L35="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>$L35="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="39" priority="1">
       <formula>$L56="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="38" priority="2">
       <formula>$L56="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="37" priority="3">
       <formula>$L56="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="36" priority="4">
       <formula>$L56="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="35" priority="5">
       <formula>$L56="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="34" priority="6">
       <formula>$L56="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="33" priority="7">
       <formula>$L56="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="32" priority="8">
       <formula>$L56="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14192,106 +14192,106 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A104">
-    <cfRule type="expression" dxfId="767" priority="41">
+    <cfRule type="expression" dxfId="31" priority="41">
       <formula>$D1="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="766" priority="42">
+    <cfRule type="expression" dxfId="30" priority="42">
       <formula>$D1="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="765" priority="43">
+    <cfRule type="expression" dxfId="29" priority="43">
       <formula>$D1="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="764" priority="44">
+    <cfRule type="expression" dxfId="28" priority="44">
       <formula>$D1="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="763" priority="45">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>$D1="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="762" priority="46">
+    <cfRule type="expression" dxfId="26" priority="46">
       <formula>$D1="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="761" priority="47">
+    <cfRule type="expression" dxfId="25" priority="47">
       <formula>$D1="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="760" priority="48">
+    <cfRule type="expression" dxfId="24" priority="48">
       <formula>$D1="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:A111">
-    <cfRule type="expression" dxfId="759" priority="33">
+    <cfRule type="expression" dxfId="23" priority="33">
       <formula>$D105="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="758" priority="34">
+    <cfRule type="expression" dxfId="22" priority="34">
       <formula>$D105="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="757" priority="35">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>$D105="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="756" priority="36">
+    <cfRule type="expression" dxfId="20" priority="36">
       <formula>$D105="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="755" priority="37">
+    <cfRule type="expression" dxfId="19" priority="37">
       <formula>$D105="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="754" priority="38">
+    <cfRule type="expression" dxfId="18" priority="38">
       <formula>$D105="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="753" priority="39">
+    <cfRule type="expression" dxfId="17" priority="39">
       <formula>$D105="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="752" priority="40">
+    <cfRule type="expression" dxfId="16" priority="40">
       <formula>$D105="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B104">
-    <cfRule type="expression" dxfId="751" priority="9">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>$D1="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="750" priority="10">
+    <cfRule type="expression" dxfId="14" priority="10">
       <formula>$D1="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="749" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>$D1="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="748" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>$D1="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="747" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>$D1="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="746" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>$D1="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="745" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>$D1="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="744" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>$D1="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105:B111">
-    <cfRule type="expression" dxfId="743" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$D105="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="742" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$D105="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="741" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$D105="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="740" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$D105="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="739" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$D105="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="738" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$D105="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="737" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$D105="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="736" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$D105="Failed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Smoke script files
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Script Fixing\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite_BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7590" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="420">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -1276,6 +1276,24 @@
   </si>
   <si>
     <t>2020-08: CH1-TGL</t>
+  </si>
+  <si>
+    <t>JobCreation_2</t>
+  </si>
+  <si>
+    <t>CreateBudget_2</t>
+  </si>
+  <si>
+    <t>CreateQuote_2</t>
+  </si>
+  <si>
+    <t>CRT-748</t>
+  </si>
+  <si>
+    <t>2020-09: CH1-HC1</t>
+  </si>
+  <si>
+    <t>CRT-755</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1505,12 +1523,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1562,6 +1593,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8086,8 +8120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8109,7 +8143,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8125,7 +8159,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -8141,7 +8175,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>1707</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8196,10 +8230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8207,6 +8241,7 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8270,6 +8305,11 @@
       </c>
       <c r="D4" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -8283,7 +8323,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8335,6 +8375,9 @@
       <c r="E3">
         <v>1008</v>
       </c>
+      <c r="F3">
+        <v>2031</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -8342,6 +8385,9 @@
       </c>
       <c r="B4">
         <v>1322</v>
+      </c>
+      <c r="E4">
+        <v>1003</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8362,19 +8408,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -8387,11 +8434,14 @@
       <c r="D1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
@@ -8404,11 +8454,14 @@
       <c r="D2" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="31" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="19" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -8425,7 +8478,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -8442,7 +8495,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -8459,7 +8512,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -8476,7 +8529,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -8493,7 +8546,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -8509,8 +8562,11 @@
       <c r="E8" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -8527,7 +8583,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -8544,7 +8600,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -8561,7 +8617,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -8578,7 +8634,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -8595,7 +8651,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -8612,7 +8668,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -8629,7 +8685,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -9190,7 +9246,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -9207,7 +9263,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -9224,7 +9280,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -9241,7 +9297,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -9258,7 +9314,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -9275,7 +9331,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -9292,7 +9348,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -9309,7 +9365,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>172</v>
       </c>
@@ -9326,7 +9382,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -9343,7 +9399,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -9360,7 +9416,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>103</v>
       </c>
@@ -9377,7 +9433,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -9394,7 +9450,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>105</v>
       </c>
@@ -9410,8 +9466,11 @@
       <c r="E61" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>106</v>
       </c>
@@ -9428,7 +9487,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>107</v>
       </c>
@@ -9445,7 +9504,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>108</v>
       </c>
@@ -10210,8 +10269,31 @@
         <v>412</v>
       </c>
     </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>414</v>
+      </c>
+      <c r="E109" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="E110" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>416</v>
+      </c>
+      <c r="E111" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E100"/>
   <conditionalFormatting sqref="B3">
     <cfRule type="expression" dxfId="767" priority="729">
       <formula>$L3="Passed"</formula>
@@ -14435,15 +14517,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -14640,6 +14713,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -14647,14 +14729,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E10866D-5BB4-44E5-B346-014C2F2BBDD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14669,6 +14743,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating JIRA Ids for JAN Regression
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/EnvParamaters.xlsx
+++ b/WppRegpack/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Jan Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\GlobalTestSuite Project\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7590" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EnvDetails" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="331">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -2882,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5988,7 +5988,7 @@
   <dimension ref="A1:G462"/>
   <sheetViews>
     <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G110"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9952,10 +9952,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9965,7 +9965,7 @@
     <col min="3" max="4" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -9978,8 +9978,11 @@
       <c r="D1" s="17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -9993,7 +9996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
@@ -10007,7 +10010,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
@@ -10033,18 +10036,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10245,26 +10248,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4497BB-2D29-4E82-A8DD-4A16B586A2A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87386783-DDA8-4D9D-9418-1E12D68F1355}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b437d513-bcd3-4295-b540-77b94a32e6f7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>